<commit_message>
Refactorizaciones como comentarios en el código de cada clase
</commit_message>
<xml_diff>
--- a/Metricas de Producto.xlsx
+++ b/Metricas de Producto.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickl\Desktop\Ingeniería_Informática\3rd_year_round2\2nd_semester\SW2\Practicas\IS2_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1E298B-CA46-4750-913C-EDF45AF98614}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F33ED05-CC3D-413D-A443-963592CDE6B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>WMC</t>
   </si>
@@ -76,27 +85,6 @@
   </si>
   <si>
     <t>CCog</t>
-  </si>
-  <si>
-    <t>n=4</t>
-  </si>
-  <si>
-    <t>n=3</t>
-  </si>
-  <si>
-    <t>n=9</t>
-  </si>
-  <si>
-    <t>n=2</t>
-  </si>
-  <si>
-    <t>n=6</t>
-  </si>
-  <si>
-    <t>n=11</t>
-  </si>
-  <si>
-    <t>n=1</t>
   </si>
   <si>
     <t>1
@@ -160,6 +148,9 @@
 Cuenta
 CuentaAhorro
 CuentaValores</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -242,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -256,9 +247,7 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -545,375 +534,442 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:N16"/>
+  <dimension ref="A3:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" customWidth="1"/>
     <col min="11" max="11" width="33.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="3" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="4"/>
+      <c r="J3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="4"/>
+      <c r="L3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4"/>
+      <c r="N3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
+      <c r="O3" s="4"/>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="I4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="K4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="M4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="O4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="7">
+        <f>D5/B5</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="7" t="e">
+        <f>E5/C5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8">
+        <v>0</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7">
+        <v>8</v>
+      </c>
+      <c r="O5" s="7"/>
+    </row>
+    <row r="6" spans="1:15" ht="210" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7">
+        <f>D6/B6</f>
+        <v>1.7777777777777777</v>
+      </c>
+      <c r="G6" s="7" t="e">
+        <f>E6/C6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8">
+        <v>0</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7">
+        <v>7</v>
+      </c>
+      <c r="O6" s="7"/>
+    </row>
+    <row r="7" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="7">
+        <f t="shared" ref="F7:F13" si="0">D7/B7</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="7" t="e">
+        <f t="shared" ref="G7:G13" si="1">E7/C7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8">
+        <v>2</v>
+      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7">
+        <v>0</v>
+      </c>
+      <c r="O7" s="7"/>
+    </row>
+    <row r="8" spans="1:15" ht="225" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1">
+        <v>13</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="0"/>
+        <v>1.6363636363636365</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" si="1"/>
+        <v>1.4444444444444444</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="8"/>
+      <c r="L8" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7">
+        <v>7</v>
+      </c>
+      <c r="O8" s="7"/>
+    </row>
+    <row r="9" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8">
+        <v>0</v>
+      </c>
+      <c r="K9" s="8"/>
+      <c r="L9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7">
+        <v>0</v>
+      </c>
+      <c r="O9" s="7"/>
+    </row>
+    <row r="10" spans="1:15" ht="165" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="G10" s="7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8">
+        <v>0</v>
+      </c>
+      <c r="K10" s="8"/>
+      <c r="L10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7">
+        <v>2</v>
+      </c>
+      <c r="O10" s="7"/>
+    </row>
+    <row r="11" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1">
+        <v>6</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G11" s="7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8">
+        <v>0</v>
+      </c>
+      <c r="K11" s="8"/>
+      <c r="L11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7">
+        <v>0</v>
+      </c>
+      <c r="O11" s="7"/>
+    </row>
+    <row r="12" spans="1:15" ht="180" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="9">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G12" s="7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8">
+        <v>2</v>
+      </c>
+      <c r="K12" s="8"/>
+      <c r="L12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7">
+        <v>0</v>
+      </c>
+      <c r="O12" s="7"/>
+    </row>
+    <row r="13" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="1">
+        <v>6</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G13" s="7" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8">
+        <v>0</v>
+      </c>
+      <c r="K13" s="8"/>
+      <c r="L13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="7">
-        <v>2</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8">
-        <v>0</v>
-      </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7">
-        <v>8</v>
-      </c>
-      <c r="N5" s="7"/>
-    </row>
-    <row r="6" spans="1:14" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1">
-        <v>16</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="7">
-        <v>1.7777777777777777</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="8">
-        <v>1</v>
-      </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8">
-        <v>0</v>
-      </c>
-      <c r="J6" s="8"/>
-      <c r="K6" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7">
-        <v>7</v>
-      </c>
-      <c r="N6" s="7"/>
-    </row>
-    <row r="7" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="8">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8">
-        <v>2</v>
-      </c>
-      <c r="J7" s="8"/>
-      <c r="K7" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7">
-        <v>0</v>
-      </c>
-      <c r="N7" s="7"/>
-    </row>
-    <row r="8" spans="1:14" ht="135" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="7">
-        <v>1.6363636363636365</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8">
-        <v>0</v>
-      </c>
-      <c r="J8" s="8"/>
-      <c r="K8" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7">
-        <v>7</v>
-      </c>
-      <c r="N8" s="7"/>
-    </row>
-    <row r="9" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1">
-        <v>3</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="7">
-        <v>1</v>
-      </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8">
-        <v>1</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8">
-        <v>0</v>
-      </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7">
-        <v>0</v>
-      </c>
-      <c r="N9" s="7"/>
-    </row>
-    <row r="10" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1">
-        <v>8</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="7">
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8">
-        <v>1</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8">
-        <v>0</v>
-      </c>
-      <c r="J10" s="8"/>
-      <c r="K10" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7">
-        <v>2</v>
-      </c>
-      <c r="N10" s="7"/>
-    </row>
-    <row r="11" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1">
-        <v>6</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="7">
-        <v>1</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8">
-        <v>0</v>
-      </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8">
-        <v>0</v>
-      </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7">
-        <v>0</v>
-      </c>
-      <c r="N11" s="7"/>
-    </row>
-    <row r="12" spans="1:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="10">
-        <v>1</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="9">
-        <v>1</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8">
-        <v>0</v>
-      </c>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8">
-        <v>2</v>
-      </c>
-      <c r="J12" s="8"/>
-      <c r="K12" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7">
-        <v>0</v>
-      </c>
-      <c r="N12" s="7"/>
-    </row>
-    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1">
-        <v>6</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="7">
-        <v>1</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8">
-        <v>0</v>
-      </c>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8">
-        <v>0</v>
-      </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7">
-        <v>0</v>
-      </c>
-      <c r="N13" s="7"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M13" s="7"/>
+      <c r="N13" s="7">
+        <v>0</v>
+      </c>
+      <c r="O13" s="7"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -928,7 +984,7 @@
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -943,7 +999,7 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>

</xml_diff>

<commit_message>
Tabla de metricas completada
</commit_message>
<xml_diff>
--- a/Metricas de Producto.xlsx
+++ b/Metricas de Producto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickl\Desktop\Ingeniería_Informática\3rd_year_round2\2nd_semester\SW2\Practicas\IS2_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F33ED05-CC3D-413D-A443-963592CDE6B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49374207-DCFA-4925-AFA3-E12D2E263993}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>WMC</t>
   </si>
@@ -85,10 +85,6 @@
   </si>
   <si>
     <t>CCog</t>
-  </si>
-  <si>
-    <t>1
-CuentaValores</t>
   </si>
   <si>
     <t>5
@@ -144,13 +140,37 @@
 Cuenta</t>
   </si>
   <si>
-    <t>3
+    <t>n</t>
+  </si>
+  <si>
+    <t>Direccion</t>
+  </si>
+  <si>
+    <t>1
+Cliente</t>
+  </si>
+  <si>
+    <t>4
 Cuenta
 CuentaAhorro
-CuentaValores</t>
-  </si>
-  <si>
-    <t>n</t>
+CuentaValores
+Valor</t>
+  </si>
+  <si>
+    <t>5
+Cuenta
+CuentaAhorro
+CuentaValores
+Valor
+Direccion</t>
+  </si>
+  <si>
+    <t>2
+CuentaValores
+Cliente</t>
+  </si>
+  <si>
+    <t>Clases</t>
   </si>
 </sst>
 </file>
@@ -233,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -252,6 +272,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -537,21 +564,31 @@
   <dimension ref="A3:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="11" max="11" width="33.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="3" width="6.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="5" max="5" width="6" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="7" max="7" width="7" customWidth="1"/>
+    <col min="8" max="8" width="5.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" customWidth="1"/>
+    <col min="10" max="10" width="5.140625" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" customWidth="1"/>
+    <col min="12" max="12" width="26.28515625" customWidth="1"/>
+    <col min="13" max="13" width="24.85546875" customWidth="1"/>
+    <col min="14" max="14" width="6.85546875" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="5" t="s">
@@ -580,7 +617,9 @@
       <c r="O3" s="4"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -624,44 +663,56 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>5</v>
+      </c>
       <c r="D5" s="1">
         <v>8</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1">
+        <v>9</v>
+      </c>
       <c r="F5" s="7">
         <f>D5/B5</f>
         <v>2</v>
       </c>
-      <c r="G5" s="7" t="e">
+      <c r="G5" s="7">
         <f>E5/C5</f>
-        <v>#DIV/0!</v>
+        <v>1.8</v>
       </c>
       <c r="H5" s="8">
         <v>0</v>
       </c>
-      <c r="I5" s="8"/>
+      <c r="I5" s="8">
+        <v>0</v>
+      </c>
       <c r="J5" s="8">
         <v>0</v>
       </c>
-      <c r="K5" s="8"/>
+      <c r="K5" s="8">
+        <v>0</v>
+      </c>
       <c r="L5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7">
+        <v>27</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="12">
         <v>8</v>
       </c>
-      <c r="O5" s="7"/>
-    </row>
-    <row r="6" spans="1:15" ht="210" x14ac:dyDescent="0.25">
+      <c r="O5" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -669,77 +720,97 @@
         <v>9</v>
       </c>
       <c r="C6" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1">
         <v>16</v>
       </c>
       <c r="E6" s="1">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F6" s="7">
         <f>D6/B6</f>
         <v>1.7777777777777777</v>
       </c>
-      <c r="G6" s="7" t="e">
+      <c r="G6" s="7">
         <f>E6/C6</f>
-        <v>#DIV/0!</v>
+        <v>1.4545454545454546</v>
       </c>
       <c r="H6" s="8">
         <v>1</v>
       </c>
-      <c r="I6" s="8"/>
+      <c r="I6" s="8">
+        <v>1</v>
+      </c>
       <c r="J6" s="8">
         <v>0</v>
       </c>
-      <c r="K6" s="8"/>
+      <c r="K6" s="8">
+        <v>0</v>
+      </c>
       <c r="L6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7">
+        <v>23</v>
+      </c>
+      <c r="M6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="12">
         <v>7</v>
       </c>
-      <c r="O6" s="7"/>
-    </row>
-    <row r="7" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+      <c r="O6" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
       <c r="D7" s="1">
         <v>2</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
       <c r="F7" s="7">
         <f t="shared" ref="F7:F13" si="0">D7/B7</f>
         <v>1</v>
       </c>
-      <c r="G7" s="7" t="e">
-        <f t="shared" ref="G7:G13" si="1">E7/C7</f>
-        <v>#DIV/0!</v>
+      <c r="G7" s="7">
+        <f t="shared" ref="G7:G14" si="1">E7/C7</f>
+        <v>1</v>
       </c>
       <c r="H7" s="8">
         <v>0</v>
       </c>
-      <c r="I7" s="8"/>
+      <c r="I7" s="8">
+        <v>0</v>
+      </c>
       <c r="J7" s="8">
         <v>2</v>
       </c>
-      <c r="K7" s="8"/>
+      <c r="K7" s="8">
+        <v>2</v>
+      </c>
       <c r="L7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7">
-        <v>0</v>
-      </c>
-      <c r="O7" s="7"/>
-    </row>
-    <row r="8" spans="1:15" ht="225" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="12">
+        <v>0</v>
+      </c>
+      <c r="O7" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -747,13 +818,13 @@
         <v>11</v>
       </c>
       <c r="C8" s="1">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1">
         <v>18</v>
       </c>
       <c r="E8" s="1">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="0"/>
@@ -761,24 +832,32 @@
       </c>
       <c r="G8" s="7">
         <f t="shared" si="1"/>
-        <v>1.4444444444444444</v>
+        <v>1.2857142857142858</v>
       </c>
       <c r="H8" s="8">
         <v>1</v>
       </c>
-      <c r="I8" s="8"/>
+      <c r="I8" s="8">
+        <v>1</v>
+      </c>
       <c r="J8" s="8">
         <v>0</v>
       </c>
-      <c r="K8" s="8"/>
+      <c r="K8" s="8">
+        <v>0</v>
+      </c>
       <c r="L8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7">
+        <v>21</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="12">
         <v>7</v>
       </c>
-      <c r="O8" s="7"/>
+      <c r="O8" s="12">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -787,37 +866,49 @@
       <c r="B9" s="1">
         <v>3</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
       <c r="D9" s="1">
         <v>3</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
       <c r="F9" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G9" s="7" t="e">
+      <c r="G9" s="7">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="H9" s="8">
         <v>1</v>
       </c>
-      <c r="I9" s="8"/>
+      <c r="I9" s="8">
+        <v>1</v>
+      </c>
       <c r="J9" s="8">
         <v>0</v>
       </c>
-      <c r="K9" s="8"/>
+      <c r="K9" s="8">
+        <v>0</v>
+      </c>
       <c r="L9" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7">
-        <v>0</v>
-      </c>
-      <c r="O9" s="7"/>
-    </row>
-    <row r="10" spans="1:15" ht="165" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="12">
+        <v>0</v>
+      </c>
+      <c r="O9" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -825,164 +916,227 @@
         <v>6</v>
       </c>
       <c r="C10" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D10" s="1">
         <v>8</v>
       </c>
       <c r="E10" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
-      <c r="G10" s="7" t="e">
+      <c r="G10" s="7">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1.1428571428571428</v>
       </c>
       <c r="H10" s="8">
         <v>1</v>
       </c>
-      <c r="I10" s="8"/>
+      <c r="I10" s="8">
+        <v>1</v>
+      </c>
       <c r="J10" s="8">
         <v>0</v>
       </c>
-      <c r="K10" s="8"/>
+      <c r="K10" s="8">
+        <v>0</v>
+      </c>
       <c r="L10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7">
+        <v>19</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="12">
         <v>2</v>
       </c>
-      <c r="O10" s="7"/>
-    </row>
-    <row r="11" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="O10" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="1">
         <v>6</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>6</v>
+      </c>
       <c r="D11" s="1">
         <v>6</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1">
+        <v>6</v>
+      </c>
       <c r="F11" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G11" s="7" t="e">
+      <c r="G11" s="7">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="H11" s="8">
         <v>0</v>
       </c>
-      <c r="I11" s="8"/>
+      <c r="I11" s="8">
+        <v>0</v>
+      </c>
       <c r="J11" s="8">
         <v>0</v>
       </c>
-      <c r="K11" s="8"/>
+      <c r="K11" s="8">
+        <v>0</v>
+      </c>
       <c r="L11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7">
-        <v>0</v>
-      </c>
-      <c r="O11" s="7"/>
-    </row>
-    <row r="12" spans="1:15" ht="180" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="12">
+        <v>0</v>
+      </c>
+      <c r="O11" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="9">
         <v>1</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
       <c r="D12" s="9">
         <v>1</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
       <c r="F12" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G12" s="7" t="e">
+      <c r="G12" s="7">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="H12" s="8">
         <v>0</v>
       </c>
-      <c r="I12" s="8"/>
+      <c r="I12" s="8">
+        <v>0</v>
+      </c>
       <c r="J12" s="8">
         <v>2</v>
       </c>
-      <c r="K12" s="8"/>
+      <c r="K12" s="8">
+        <v>2</v>
+      </c>
       <c r="L12" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7">
-        <v>0</v>
-      </c>
-      <c r="O12" s="7"/>
-    </row>
-    <row r="13" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="12">
+        <v>0</v>
+      </c>
+      <c r="O12" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="1">
         <v>6</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1">
+        <v>6</v>
+      </c>
       <c r="D13" s="1">
         <v>6</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1">
+        <v>6</v>
+      </c>
       <c r="F13" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G13" s="7" t="e">
+      <c r="G13" s="7">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="H13" s="8">
         <v>0</v>
       </c>
-      <c r="I13" s="8"/>
+      <c r="I13" s="8">
+        <v>0</v>
+      </c>
       <c r="J13" s="8">
         <v>0</v>
       </c>
-      <c r="K13" s="8"/>
+      <c r="K13" s="8">
+        <v>0</v>
+      </c>
       <c r="L13" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7">
-        <v>0</v>
-      </c>
-      <c r="O13" s="7"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" s="12">
+        <v>0</v>
+      </c>
+      <c r="O13" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13">
+        <v>7</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="13">
+        <v>7</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="N14" s="1"/>
+      <c r="O14" s="15">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>

</xml_diff>

<commit_message>
Metricas de Producto actualizadas
</commit_message>
<xml_diff>
--- a/Metricas de Producto.xlsx
+++ b/Metricas de Producto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickl\Desktop\Ingeniería_Informática\3rd_year_round2\2nd_semester\SW2\Practicas\IS2_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49374207-DCFA-4925-AFA3-E12D2E263993}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDA56B0-6426-4F82-8A4D-0278B7E9B570}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:O16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>